<commit_message>
Added a new viability reagent kit
Closes #76
</commit_message>
<xml_diff>
--- a/cytof/latest/cytof.xlsx
+++ b/cytof/latest/cytof.xlsx
@@ -1,269 +1,137 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josefhardi/Documents/Code/dataset-metadata-spreadsheet/cytof/latest/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75669C0-A422-5246-AB11-B29D3347E831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CyTOF" sheetId="1" r:id="rId1"/>
-    <sheet name="dataset_type" sheetId="2" r:id="rId2"/>
-    <sheet name="analyte_class" sheetId="3" r:id="rId3"/>
-    <sheet name="is_targeted" sheetId="4" r:id="rId4"/>
-    <sheet name="acquisition_instrument_vendor" sheetId="5" r:id="rId5"/>
-    <sheet name="acquisition_instrument_model" sheetId="6" r:id="rId6"/>
-    <sheet name="source_storage_duration_unit" sheetId="7" r:id="rId7"/>
-    <sheet name="time_since_acquisition_instrume" sheetId="8" r:id="rId8"/>
-    <sheet name="is_erythrocyte_lysis_performed" sheetId="9" r:id="rId9"/>
-    <sheet name="antibody_reagent_kit" sheetId="10" r:id="rId10"/>
-    <sheet name="viability_reagent_kit" sheetId="11" r:id="rId11"/>
-    <sheet name="is_cell_activation_performed" sheetId="12" r:id="rId12"/>
-    <sheet name="is_fcr_blocking_applied" sheetId="13" r:id="rId13"/>
-    <sheet name="is_heparin_used" sheetId="14" r:id="rId14"/>
-    <sheet name="loaded_cell_concentration_unit" sheetId="15" r:id="rId15"/>
-    <sheet name="instrument_calibration_bead_kit" sheetId="16" r:id="rId16"/>
-    <sheet name=".metadata" sheetId="17" r:id="rId17"/>
+    <sheet name="CyTOF" r:id="rId3" sheetId="1"/>
+    <sheet name="dataset_type" r:id="rId4" sheetId="2"/>
+    <sheet name="analyte_class" r:id="rId5" sheetId="3"/>
+    <sheet name="is_targeted" r:id="rId6" sheetId="4"/>
+    <sheet name="acquisition_instrument_vendor" r:id="rId7" sheetId="5"/>
+    <sheet name="acquisition_instrument_model" r:id="rId8" sheetId="6"/>
+    <sheet name="source_storage_duration_unit" r:id="rId9" sheetId="7"/>
+    <sheet name="time_since_acquisition_instrume" r:id="rId10" sheetId="8"/>
+    <sheet name="is_erythrocyte_lysis_performed" r:id="rId11" sheetId="9"/>
+    <sheet name="antibody_reagent_kit" r:id="rId12" sheetId="10"/>
+    <sheet name="viability_reagent_kit" r:id="rId13" sheetId="11"/>
+    <sheet name="is_cell_activation_performed" r:id="rId14" sheetId="12"/>
+    <sheet name="is_fcr_blocking_applied" r:id="rId15" sheetId="13"/>
+    <sheet name="is_heparin_used" r:id="rId16" sheetId="14"/>
+    <sheet name="loaded_cell_concentration_unit" r:id="rId17" sheetId="15"/>
+    <sheet name="instrument_calibration_bead_kit" r:id="rId18" sheetId="16"/>
+    <sheet name=".metadata" r:id="rId19" sheetId="17"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author/>
     <author>CEDAR Metadata Validator</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
+        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
 section or suspension) used to perform this assay. For example, for a RNAseq
 assay, the parent would be the suspension, whereas, for one of the imaging
 assays, the parent would be the tissue section. If an assay comes from multiple
 parent samples then this should be a comma separated list. Example:
 HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
-        </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>An internal field labs can use it to add whatever ID(s) they want or need for
+        <t>An internal field labs can use it to add whatever ID(s) they want or need for
 dataset validation and tracking. This could be a single ID (e.g.,
 "Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
 Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
 consortium and no effort will be made to check if IDs provided by one data
 provider are also used by another.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) DOI for the protocols.io page that describes the assay or sample
+        <t>(Required) DOI for the protocols.io page that describes the assay or sample
 procurment and preparation. For example for an imaging assay, the protocol might
 include staining of a section through the creation of an OME-TIFF file. In this
 case the protocol would include any image processing steps required to create
 the OME-TIFF file. Example:
 https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
-        </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="D1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) The specific type of dataset being produced.</t>
-        </r>
+        <t>(Required) The specific type of dataset being produced.</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="E1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) Analytes are the target molecules being measured with the assay.</t>
-        </r>
+        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="F1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
+        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
 detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
 protein.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="G1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) An acquisition instrument is the device that contains the signal
+        <t>(Required) An acquisition instrument is the device that contains the signal
 detection hardware and signal processing software. Assays generate signals such
 as light of various intensities or color or signals representing the molecular
 mass.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="H1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) Manufacturers of an acquisition instrument may offer various versions
+        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
 (models) of that instrument with different features or sensitivities.
 Differences in features or sensitivities may be relevant to processing or
 interpretation of the data.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="I1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) How long was the source material stored, prior to this sample being
+        <t>(Required) How long was the source material stored, prior to this sample being
 processed? For assays applied to tissue sections, this would be how long the
 tissue section (e.g., slide) was stored, prior to the assay beginning (e.g.,
 imaging). For assays applied to suspensions such as sequencing, this would be
 how long the suspension was stored before library construction began.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="J1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) The time duration unit of measurement</t>
-        </r>
+        <t>(Required) The time duration unit of measurement</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="K1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The amount of time since the acqusition instrument was last serviced by the
+        <t>The amount of time since the acqusition instrument was last serviced by the
 vendor. This provides a metric for assessing drift in data capture.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="L1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The time unit of measurement</t>
-        </r>
+        <t>The time unit of measurement</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="M1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) The path to the file with the ORCID IDs for all contributors of this
+        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
 dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
 internal metadata field that is just used for ingest.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="N1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>(Required) The top level directory containing the raw and/or processed data. For
+        <t>(Required) The top level directory containing the raw and/or processed data. For
 a single dataset upload this might be "." where as for a data upload containing
 multiple datasets, this would be the directory name for the respective dataset.
 For instance, if the data is within a directory called "TEST001-RK" use syntax
@@ -271,214 +139,96 @@
 format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
 single dataset's data is stored. This is an internal metadata field that is just
 used for ingest.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="O1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The number of mass channels that measure the expression of markers in single
+        <t>The number of mass channels that measure the expression of markers in single
 cells.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="P1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Process in which red blood cells (RBCs) are broken down in the sample prior to
+        <t>Process in which red blood cells (RBCs) are broken down in the sample prior to
 analysis, thereby allowing researchers to focus primarily on white blood cells
 (WBCs).</t>
-        </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="Q1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The kit containing the set of antibodies pre-conjugated with different heavy
+        <t>The kit containing the set of antibodies pre-conjugated with different heavy
 metal isotopes used to simultaneously detect and quantify multiple protein
 markers on individual cells by attaching these metal-labeled antibodies to
 specific cellular targets, essentially acting as the key component for labeling
 cells with the various markers needed for analysis on the CyTOF machine.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="R1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The kit used to differentiate between live and dead cells within a sample by
+        <t>The kit used to differentiate between live and dead cells within a sample by
 selectively staining dead cells with a dye that can be detected by the
 instrument, allowing researchers to exclude dead cell data from their analysis
 and ensure accurate results when studying cell populations.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="S1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Process by which ligand is binded to its receptors on a cell, which enhances the
+        <t>Process by which ligand is binded to its receptors on a cell, which enhances the
 cell's ability to respond to various stimuli.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="T1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Specific type of stimulus used to provoke cell activation. Examples would
+        <t>Specific type of stimulus used to provoke cell activation. Examples would
 include PMA/ionomycin or CD28in/brefeldin A. This field is required if
 "is_cells_activation performed" is Yes.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="U1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Process by which a reagent has been added to the staining procedure to block the
+        <t>Process by which a reagent has been added to the staining procedure to block the
 binding of antibodies to Fc receptors (FcRs) on cells, preventing non-specific
 binding and ensuring that only the intended target antigen is detected by the
 antibodies; essentially, it helps to minimize false positive signals by
 preventing antibodies from attaching to the cell via their Fc region instead of
 the antigen-specific binding site.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="V1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Indicates whether heparin was used ("Yes") or not ("No") during staining to
+        <t>Indicates whether heparin was used ("Yes") or not ("No") during staining to
 prevent non-specific binding of metal-labeled antibodies to eosinophils to
 reduce background noise.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="W1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The number of cells present within a given volume of liquid for the experiment
+        <t>The number of cells present within a given volume of liquid for the experiment
 immediately prior to the experiment, essentially indicating how densely packed
 the cells are in a solution.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="X1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Unit of measure for cell concentration, e.g. cells per milliliter (cells/mL).</t>
-        </r>
+        <t>Unit of measure for cell concentration, e.g. cells per milliliter (cells/mL).</t>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+    <comment ref="Y1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>A set of beads of known mass intensity used to adjust the settings of a flow
+        <t>A set of beads of known mass intensity used to adjust the settings of a flow
 cytometer to ensure accurate measurements.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
+    <comment ref="Z1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Manufacturer's lot number for the calibration bead kit used for the experiment.</t>
-        </r>
+        <t>Manufacturer's lot number for the calibration bead kit used for the experiment.</t>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+    <comment ref="AA1" authorId="1">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The string that serves as the definitive identifier for the metadata schema
+        <t>The string that serves as the definitive identifier for the metadata schema
 version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -486,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="369">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1472,39 +1222,48 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000417</t>
   </si>
   <si>
+    <t>Standard BioTools; Cell-ID Cisplatin 100 uL; PN 201064</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000412</t>
+  </si>
+  <si>
+    <t>Standard BioTools; Cell-ID Cisplatin-194Pt 100 uL; PN 201194</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000413</t>
+  </si>
+  <si>
+    <t>Sigma Aldrich; Cisplatin 25mg; PN P4394</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000419</t>
+  </si>
+  <si>
+    <t>Standard BioTools; Cell-ID Cisplatin-196Pt 100 uL; PN 201196</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000415</t>
+  </si>
+  <si>
+    <t>Standard BioTools; Cell-ID Intercalator-103Rh 2,000 um; PN 201103B</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000418</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C41132</t>
+  </si>
+  <si>
+    <t>Standard BioTools; Cell-ID Cisplatin-198Pt 100 uL; PN 201198</t>
+  </si>
+  <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000416</t>
   </si>
   <si>
-    <t>Standard BioTools; Cell-ID Cisplatin 100 uL; PN 201064</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000412</t>
-  </si>
-  <si>
-    <t>Standard BioTools; Cell-ID Cisplatin-194Pt 100 uL; PN 201194</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000413</t>
-  </si>
-  <si>
-    <t>Standard BioTools; Cell-ID Cisplatin-196Pt 100 uL; PN 201196</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000415</t>
-  </si>
-  <si>
-    <t>Standard BioTools; Cell-ID Intercalator-103Rh 2,000 um; PN 201103B</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000418</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C41132</t>
-  </si>
-  <si>
     <t>Standard BioTools; Cell-ID Cisplatin-195Pt 100 uL; PN 201195</t>
   </si>
   <si>
@@ -1577,37 +1336,45 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-03-11T07:42:12-07:00</t>
+    <t>2025-03-11T19:32:42-04:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
   </si>
   <si>
     <t>https://repo.metadatacenter.org/templates/4cb5ad9a-e5cc-4c3f-98cd-e685330165a9</t>
-  </si>
-  <si>
-    <t>Standard BioTools; Cell-ID Cisplatin-198Pt 100 uL; PN 201198</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=""/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1628,2238 +1395,1908 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="0E2841"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="156082"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="E97132"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="196B24"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="A02B93"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="4EA72E"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="467886"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="96607D"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="41.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="14.39453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="5.46875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="4" width="20.234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="5" width="10.59765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="10.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="7" width="9.40234375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="8" width="24.5546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="9" width="24.0390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="10" width="24.63671875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="11" width="23.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="12" width="41.1015625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="13" width="40.1015625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="14" width="14.5859375" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" style="15" width="8.46484375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" style="16" width="21.5234375" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" style="17" width="24.62109375" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="16.98828125" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" style="19" width="16.23046875" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="22.64453125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="15.67578125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" style="22" width="18.8125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" style="23" width="13.2265625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" style="24" width="25.61328125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" style="25" width="24.61328125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" style="26" width="25.5" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" style="27" width="21.34375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" style="28" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s" s="1">
         <v>84</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s" s="1">
         <v>117</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s" s="1">
         <v>120</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s" s="1">
         <v>169</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s" s="1">
         <v>296</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s" s="1">
         <v>297</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s" s="1">
         <v>308</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s" s="1">
         <v>309</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s" s="1">
         <v>310</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s" s="1">
         <v>311</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s" s="1">
         <v>312</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s" s="1">
         <v>313</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s" s="1">
         <v>314</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s" s="1">
         <v>325</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="S1" t="s" s="1">
         <v>344</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="T1" t="s" s="1">
         <v>345</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="U1" t="s" s="1">
         <v>346</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="V1" t="s" s="1">
+        <v>347</v>
+      </c>
+      <c r="W1" t="s" s="1">
+        <v>348</v>
+      </c>
+      <c r="X1" t="s" s="1">
         <v>349</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D2" t="s">
+      <c r="Y1" t="s" s="1">
+        <v>352</v>
+      </c>
+      <c r="Z1" t="s" s="1">
+        <v>359</v>
+      </c>
+      <c r="AA1" t="s" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="D2" t="s" s="5">
         <v>82</v>
       </c>
-      <c r="AA2" t="s">
-        <v>358</v>
+      <c r="AA2" t="s" s="28">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" error="Value should be greater than 0" sqref="I2:I1001 K2:K1001" xr:uid="{00000000-0002-0000-0000-000005000000}">
+  <dataValidations count="19">
+    <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'dataset_type'!$A$1:$A$40</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'analyte_class'!$A$1:$A$16</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'is_targeted'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$24</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'acquisition_instrument_model'!$A$1:$A$63</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
+      <formula2/>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" error="Value should be a number" sqref="O2:O1001 W2:W1001" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'source_storage_duration_unit'!$A$1:$A$5</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
+      <formula1>0</formula1>
+      <formula2/>
+    </dataValidation>
+    <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="between" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-2147483648</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
+    <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'is_erythrocyte_lysis_performed'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'antibody_reagent_kit'!$A$1:$A$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'viability_reagent_kit'!$A$1:$A$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'is_cell_activation_performed'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'is_fcr_blocking_applied'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="V2:V1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'is_heparin_used'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="between" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
+      <formula1>-2147483648</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'loaded_cell_concentration_unit'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="Y2:Y1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'instrument_calibration_bead_kit'!$A$1:$A$5</formula1>
+    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>dataset_type!$A$1:$A$40</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>analyte_class!$A$1:$A$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>is_targeted!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>acquisition_instrument_vendor!$A$1:$A$24</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>acquisition_instrument_model!$A$1:$A$63</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000006000000}">
-          <x14:formula1>
-            <xm:f>source_storage_duration_unit!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000008000000}">
-          <x14:formula1>
-            <xm:f>time_since_acquisition_instrume!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>L2:L1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000A000000}">
-          <x14:formula1>
-            <xm:f>is_erythrocyte_lysis_performed!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>P2:P1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000B000000}">
-          <x14:formula1>
-            <xm:f>antibody_reagent_kit!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000C000000}">
-          <x14:formula1>
-            <xm:f>viability_reagent_kit!$A$1:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>R2:R1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000D000000}">
-          <x14:formula1>
-            <xm:f>is_cell_activation_performed!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>S2:S1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000E000000}">
-          <x14:formula1>
-            <xm:f>is_fcr_blocking_applied!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>U2:U1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-00000F000000}">
-          <x14:formula1>
-            <xm:f>is_heparin_used!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>V2:V1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000011000000}">
-          <x14:formula1>
-            <xm:f>loaded_cell_concentration_unit!$A$1:$A$1</xm:f>
-          </x14:formula1>
-          <xm:sqref>X2:X1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Validation Error" xr:uid="{00000000-0002-0000-0000-000012000000}">
-          <x14:formula1>
-            <xm:f>instrument_calibration_bead_kit!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>Y2:Y1001</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>317</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>319</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>320</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>321</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>323</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>324</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>326</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>328</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B2" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>330</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B3" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>332</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>319</v>
-      </c>
-      <c r="B5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B5" t="s" s="0">
         <v>333</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>334</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B6" t="s" s="0">
         <v>335</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
         <v>336</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" t="s" s="0">
         <v>337</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>338</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B8" t="s" s="0">
         <v>339</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>340</v>
       </c>
+      <c r="B9" t="s" s="0">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>342</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>343</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B1" t="s">
-        <v>348</v>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>353</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B1" t="s" s="0">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>355</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>319</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>320</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B4" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>357</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>338</v>
       </c>
+      <c r="B5" t="s" s="0">
+        <v>339</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.20703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="68.9453125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" t="s" s="0">
+        <v>363</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>364</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C2" t="s">
-        <v>363</v>
-      </c>
-      <c r="D2" t="s">
-        <v>365</v>
+      <c r="C2" t="s" s="0">
+        <v>366</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21">
+      <c r="A21" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22">
+      <c r="A22" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23">
+      <c r="A23" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24">
+      <c r="A24" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25">
+      <c r="A25" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26">
+      <c r="A26" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27">
+      <c r="A27" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28">
+      <c r="A28" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29">
+      <c r="A29" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30">
+      <c r="A30" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31">
+      <c r="A31" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32">
+      <c r="A32" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33">
+      <c r="A33" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34">
+      <c r="A34" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35">
+      <c r="A35" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36">
+      <c r="A36" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37">
+      <c r="A37" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38">
+      <c r="A38" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39">
+      <c r="A39" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40">
+      <c r="A40" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>116</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" t="s" s="0">
         <v>157</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21">
+      <c r="A21" t="s" s="0">
         <v>161</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22">
+      <c r="A22" t="s" s="0">
         <v>163</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23">
+      <c r="A23" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24">
+      <c r="A24" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>172</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" t="s" s="0">
         <v>188</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" t="s" s="0">
         <v>190</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21">
+      <c r="A21" t="s" s="0">
         <v>210</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22">
+      <c r="A22" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23">
+      <c r="A23" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24">
+      <c r="A24" t="s" s="0">
         <v>216</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25">
+      <c r="A25" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26">
+      <c r="A26" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27">
+      <c r="A27" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28">
+      <c r="A28" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>225</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29">
+      <c r="A29" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30">
+      <c r="A30" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31">
+      <c r="A31" t="s" s="0">
         <v>230</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>231</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32">
+      <c r="A32" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>233</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33">
+      <c r="A33" t="s" s="0">
         <v>234</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34">
+      <c r="A34" t="s" s="0">
         <v>236</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35">
+      <c r="A35" t="s" s="0">
         <v>238</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36">
+      <c r="A36" t="s" s="0">
         <v>240</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37">
+      <c r="A37" t="s" s="0">
         <v>242</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38">
+      <c r="A38" t="s" s="0">
         <v>244</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>245</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39">
+      <c r="A39" t="s" s="0">
         <v>246</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40">
+      <c r="A40" t="s" s="0">
         <v>248</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>249</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41">
+      <c r="A41" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>251</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42">
+      <c r="A42" t="s" s="0">
         <v>252</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>253</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43">
+      <c r="A43" t="s" s="0">
         <v>254</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="s" s="0">
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44">
+      <c r="A44" t="s" s="0">
         <v>256</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" t="s" s="0">
         <v>257</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45">
+      <c r="A45" t="s" s="0">
         <v>258</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="0">
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46">
+      <c r="A46" t="s" s="0">
         <v>260</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" t="s" s="0">
         <v>261</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47">
+      <c r="A47" t="s" s="0">
         <v>262</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="s" s="0">
         <v>263</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48">
+      <c r="A48" t="s" s="0">
         <v>264</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="s" s="0">
         <v>265</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49">
+      <c r="A49" t="s" s="0">
         <v>266</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="s" s="0">
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50">
+      <c r="A50" t="s" s="0">
         <v>268</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" t="s" s="0">
         <v>269</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="51">
+      <c r="A51" t="s" s="0">
         <v>270</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" t="s" s="0">
         <v>271</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52">
+      <c r="A52" t="s" s="0">
         <v>272</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" t="s" s="0">
         <v>273</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53">
+      <c r="A53" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" t="s" s="0">
         <v>275</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54">
+      <c r="A54" t="s" s="0">
         <v>276</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" t="s" s="0">
         <v>277</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="55">
+      <c r="A55" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" t="s" s="0">
         <v>279</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56">
+      <c r="A56" t="s" s="0">
         <v>280</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" t="s" s="0">
         <v>281</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="57">
+      <c r="A57" t="s" s="0">
         <v>282</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" t="s" s="0">
         <v>283</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="58">
+      <c r="A58" t="s" s="0">
         <v>284</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="0">
         <v>285</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="59">
+      <c r="A59" t="s" s="0">
         <v>286</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="0">
         <v>287</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="60">
+      <c r="A60" t="s" s="0">
         <v>288</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="0">
         <v>289</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="61">
+      <c r="A61" t="s" s="0">
         <v>290</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="s" s="0">
         <v>291</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="62">
+      <c r="A62" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" t="s" s="0">
         <v>293</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63">
+      <c r="A63" t="s" s="0">
         <v>294</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="s" s="0">
         <v>295</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>299</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>302</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>304</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>306</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>307</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>302</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>304</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>305</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Flow Cytometry metadata templates to use field descriptions
</commit_message>
<xml_diff>
--- a/cytof/latest/cytof.xlsx
+++ b/cytof/latest/cytof.xlsx
@@ -36,199 +36,213 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material stored, prior to this sample being
-processed? For assays applied to tissue sections, this would be how long the
-tissue section (e.g., slide) was stored, prior to the assay beginning (e.g.,
-imaging). For assays applied to suspensions such as sequencing, this would be
-how long the suspension was stored before library construction began.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) The number of mass channels that measure the expression of markers in
-single cells.</t>
+        <t>(Required) The number of mass channels used to measure the expression of markers
+in single cells. Example: 45</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) Process in which red blood cells (RBCs) are broken down in the sample
-prior to analysis, thereby allowing researchers to focus primarily on white
-blood cells (WBCs).</t>
+        <t>(Required) Indicates whether erythrocyte lysis is performed, a process in which
+red blood cells (RBCs) are broken down in the sample before analysis. This step
+allows researchers to focus primarily on white blood cells (WBCs) during the
+analysis. Answer with "Yes" or "No" value. Example: Yes</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) The kit containing the set of antibodies pre-conjugated with
-different heavy metal isotopes used to simultaneously detect and quantify
-multiple protein markers on individual cells by attaching these metal-labeled
-antibodies to specific cellular targets, essentially acting as the key component
-for labeling cells with the various markers needed for analysis on the CyTOF
-machine.</t>
+        <t>(Required) The kit that contains antibodies pre-conjugated with different heavy
+metal isotopes, used to detect and quantify multiple protein markers on
+individual cells. These metal-labeled antibodies attach to specific cellular
+targets, serving as the key component for labeling cells with various markers.
+This may be necessary for analysis on the CyTOF machine. If custom antibody
+reagent kit is used then enter "Custom". Example: Standard BioTools; Maxpar
+Nuclear Antigen Staining Kit; PN 201603</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) The kit used to differentiate between live and dead cells within a
-sample by selectively staining dead cells with a dye that can be detected by the
-instrument, allowing researchers to exclude dead cell data from their analysis
-and ensure accurate results when studying cell populations.</t>
+        <t>(Required) The kit used to distinguish between live and dead cells in a sample
+by selectively staining dead cells with a detectable dye. This process enables
+researchers to exclude data from dead cells, ensuring accurate analysis of cell
+populations. If a custom reagent kit is utilized, enter "Custom". If reagent kit
+is not utilized, enter "None". Example: Standard BioTools; Cell-ID Cisplatin 100
+uL; PN 201064</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>(Required) Process by which ligand is binded to its receptors on a cell, which
-enhances the cell's ability to respond to various stimuli.</t>
+        <t>(Required) Indicates whether cell activation is performed, a process where a
+ligand binds to its receptors on a cell, enhancing the cell's ability to respond
+to various stimuli. Answer with "Yes" or "No" value. Example: Yes</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>Specific type of stimulus used to provoke cell activation. Examples would
-include PMA/ionomycin or CD28in/brefeldin A. This field is required if
-"is_cells_activation performed" is Yes.</t>
+        <t>The specific type of stimulus used to provoke cell activation. This field is
+required if "Is cells activation performed?" is marked as "Yes". Example:
+PMA/ionomycin</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>(Required) Process by which a reagent has been added to the staining procedure
-to block the binding of antibodies to Fc receptors (FcRs) on cells, preventing
-non-specific binding and ensuring that only the intended target antigen is
-detected by the antibodies; essentially, it helps to minimize false positive
-signals by preventing antibodies from attaching to the cell via their Fc region
-instead of the antigen-specific binding site.</t>
+        <t>(Required) Indicates whether a reagent has been added to the staining procedure
+to block the binding of antibodies to Fc receptors (FcRs) on cells. This process
+prevents non-specific binding and ensures that antibodies detect only the
+intended target antigen, thereby minimizing false positive signals by preventing
+antibodies from attaching to the cell via their Fc region instead of the
+antigen-specific binding site. Answer with "Yes" or "No" value. Example: Yes</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>(Required) Indicates whether heparin was used ("Yes") or not ("No") during
-staining to prevent non-specific binding of metal-labeled antibodies to
-eosinophils to reduce background noise.</t>
+        <t>(Required) Indicates whether heparin was used during the staining process to
+prevent non-specific binding of metal-labeled antibodies to eosinophils, thereby
+reducing background noise. Answer with "Yes" or "No" value. Example: Yes</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>The number of cells present within a given volume of liquid for the experiment
-immediately prior to the experiment, essentially indicating how densely packed
-the cells are in a solution.</t>
+        <t>The number of cells within a given volume of liquid immediately prior to the
+experiment, essentially indicating how densely packed the cells are in the
+solution. Example: 500000</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
       <text>
-        <t>Unit of measure for cell concentration, e.g. cells per milliliter (cells/mL).</t>
+        <t>The unit of measurement for the loaded cell concentration value. If no
+concentration is provided, this field may be left blank. Example: cells/mL</t>
       </text>
     </comment>
     <comment ref="Y1" authorId="1">
       <text>
-        <t>(Required) A set of beads of known mass intensity used to adjust the settings of
-a flow cytometer to ensure accurate measurements.</t>
+        <t>(Required) The calibration bead kit used with the instrument. These kits contain
+beads with known mass intensity used to adjust the settings of a flow cytometer
+to ensure accurate measurements. If custom bead kit was used, enter "Custom",
+otherwise if no bead kit was used, enter "None". Example: Standard BioTools;
+CyTOF Calibration Beads; PN 201073</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>Manufacturer's lot number for the calibration bead kit used for the experiment.</t>
+        <t>The manufacturer's lot number for the calibration bead kit used in the
+experiment. If no calibration bead kit was used or the lot number is unknown,
+this field may be left blank. Example: EQ18</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
-        <t>The string that serves as the definitive identifier for the metadata schema
-version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -237,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="426">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -263,36 +277,168 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
-  </si>
-  <si>
     <t>FACS</t>
   </si>
   <si>
@@ -305,36 +451,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -365,16 +481,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -383,30 +493,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -437,18 +529,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -461,12 +541,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -479,34 +553,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -1157,6 +1213,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1187,6 +1246,12 @@
     <t>https://identifiers.org/RRID:SCR_027095</t>
   </si>
   <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1199,6 +1264,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1223,6 +1294,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1445,7 +1522,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-07-01T10:54:17-07:00</t>
+    <t>2025-10-20T11:36:39-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1595,87 +1672,87 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>333</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>347</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>349</v>
+        <v>370</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>350</v>
+        <v>371</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>361</v>
+        <v>382</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>380</v>
+        <v>401</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>382</v>
+        <v>403</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>383</v>
+        <v>404</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>384</v>
+        <v>405</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>385</v>
+        <v>406</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>388</v>
+        <v>409</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>395</v>
+        <v>416</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>396</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="AA2" t="s" s="28">
-        <v>397</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="19">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$43</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1687,7 +1764,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$73</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1752,42 +1829,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>351</v>
+        <v>372</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>352</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>354</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>356</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>357</v>
+        <v>378</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>358</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>360</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -1805,82 +1882,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>362</v>
+        <v>383</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>363</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>364</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>365</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>366</v>
+        <v>387</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>367</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>356</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>368</v>
+        <v>389</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>369</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>370</v>
+        <v>391</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>371</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>372</v>
+        <v>393</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>373</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>374</v>
+        <v>395</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>375</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>377</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>378</v>
+        <v>399</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>379</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -1898,12 +1975,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1921,12 +1998,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1944,12 +2021,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1967,10 +2044,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>386</v>
+        <v>407</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>387</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -1988,42 +2065,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>389</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>390</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>391</v>
+        <v>412</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>392</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>356</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>393</v>
+        <v>414</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>394</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>374</v>
+        <v>395</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>375</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -2047,30 +2124,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>398</v>
+        <v>419</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>401</v>
+        <v>422</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>403</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>400</v>
+        <v>421</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>402</v>
+        <v>423</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>404</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -2080,7 +2157,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2428,6 +2505,62 @@
       </c>
       <c r="B43" t="s" s="0">
         <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2445,130 +2578,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2586,12 +2719,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2609,242 +2742,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>150</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>170</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>174</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>186</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2854,7 +2987,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2862,586 +2995,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>195</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>203</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>209</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>215</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>219</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>223</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>225</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>229</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>233</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>237</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>241</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>247</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>249</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>251</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>253</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>257</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>259</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>263</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>269</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>271</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>273</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>275</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>279</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>283</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>285</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>291</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>293</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>297</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>299</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>301</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>303</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>306</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>307</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>309</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>311</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>157</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>158</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>312</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>313</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>315</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>317</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>319</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>321</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>323</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>325</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>327</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>329</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>331</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3459,42 +3624,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>336</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>337</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>338</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>339</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>340</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>341</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>342</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>343</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3512,26 +3677,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>336</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>337</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>338</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>339</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>340</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>341</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3549,12 +3714,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>